<commit_message>
Rivisto script generazione dati Rimossa funzione ref_prices Sistemata funzione inventory_load
</commit_message>
<xml_diff>
--- a/data-raw/usitc.xlsx
+++ b/data-raw/usitc.xlsx
@@ -92,7 +92,7 @@
         </is>
       </c>
       <c r="B1" s="7" t="n">
-        <v>44830.46547310185</v>
+        <v>44833.218149872686</v>
       </c>
     </row>
     <row r="2">
@@ -239,7 +239,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2805300050, 2508400110, 28309015, 2508400120, 2530908050, 2604000080, 2805300020, 2844430021, 2614006020, 2517100020, 7110410010</t>
+          <t>28309010, 2805300050, 2508400110, 2508400120, 2530908050, 2604000080, 2805300020, 2844430021, 2614006020, 2517100020, 7110410010</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>2830.90.1500</t>
+          <t>2830.90.1000</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
@@ -1948,49 +1948,49 @@
         </is>
       </c>
       <c r="V12" s="3" t="n">
-        <v>1.78</v>
+        <v>2.19</v>
       </c>
       <c r="W12" s="3" t="n">
-        <v>1.74</v>
+        <v>2.96</v>
       </c>
       <c r="X12" s="3" t="n">
-        <v>1.8</v>
+        <v>3.2</v>
       </c>
       <c r="Y12" s="3" t="n">
-        <v>1.87</v>
+        <v>1.53</v>
       </c>
       <c r="Z12" s="3" t="n">
-        <v>1.77</v>
+        <v>1.28</v>
       </c>
       <c r="AA12" s="3" t="n">
-        <v>3.21</v>
+        <v>1.65</v>
       </c>
       <c r="AB12" s="3" t="n">
-        <v>3.91</v>
+        <v>4.5</v>
       </c>
       <c r="AC12" s="3" t="n">
-        <v>3.85</v>
+        <v>2.89</v>
       </c>
       <c r="AD12" s="3" t="n">
-        <v>3.57</v>
+        <v>1.52</v>
       </c>
       <c r="AE12" s="3" t="n">
-        <v>2.05</v>
+        <v>5.1</v>
       </c>
       <c r="AF12" s="3" t="n">
-        <v>3.54</v>
+        <v>1.75</v>
       </c>
       <c r="AG12" s="3" t="n">
-        <v>3.98</v>
+        <v>2.75</v>
       </c>
       <c r="AH12" s="3" t="n">
-        <v>4.41</v>
+        <v>2.35</v>
       </c>
       <c r="AI12" s="3" t="n">
-        <v>5.0</v>
+        <v>3.79</v>
       </c>
       <c r="AJ12" s="3" t="n">
-        <v>5.59</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="13">

</xml_diff>